<commit_message>
+prev year market snapshots
</commit_message>
<xml_diff>
--- a/Market_Snapshot.xlsx
+++ b/Market_Snapshot.xlsx
@@ -10,6 +10,8 @@
     <sheet name="Market Snapshot" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="IEX DAM" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="IEX Year Comparison" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="HPX Year Comparison" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="PXIL Year Comparison" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -495,7 +497,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>299967.075</t>
+          <t>323346.575</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -510,7 +512,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>74009.425</t>
+          <t>72624.25</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -525,7 +527,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>196358.475</t>
+          <t>231886.575</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -547,7 +549,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>337333.525</t>
+          <t>308025.4</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -562,7 +564,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>39610.65</t>
+          <t>46449.125</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -577,7 +579,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>214330.175</t>
+          <t>180857.45</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -599,7 +601,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>180400.395</t>
+          <t>182434.20</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -614,7 +616,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>28004.6875</t>
+          <t>23898.8475</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -629,7 +631,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>118838.72</t>
+          <t>104001.875</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -651,7 +653,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4.999493541666666666666666667</t>
+          <t>5.078972083333333333333333333</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -666,7 +668,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>5.323612083333333333333333333</t>
+          <t>5.603921458333333333333333333</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -681,7 +683,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>4.985656979166666666666666667</t>
+          <t>5.571529479166666666666666667</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -703,7 +705,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>4.650001927533057785156179952</t>
+          <t>4661.821206412914903017087805</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -718,7 +720,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3.344564054665848351280477599</t>
+          <t>4.523461626307502903644202927</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -733,7 +735,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>4.823371917502982193009147187</t>
+          <t>5.273936813374518488248408983</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -801,17 +803,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>24369</t>
+          <t>22851</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>24440.1</t>
+          <t>22092.8</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>11302.9</t>
+          <t>9904.6</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -828,22 +830,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5938.8</t>
+          <t>8840.2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4510.3</t>
+          <t>4899</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>4510.3</t>
+          <t>4877.72</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1499.16</t>
+          <t>1999.09</t>
         </is>
       </c>
     </row>
@@ -855,22 +857,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>12498.628125</t>
+          <t>13472.77395833333333333333333</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>14055.56354166666666666666667</t>
+          <t>12834.39166666666666666666667</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>7516.683125</t>
+          <t>7601.425</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4.999493541666666666666666667</t>
+          <t>5.078972083333333333333333333</t>
         </is>
       </c>
     </row>
@@ -901,7 +903,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Avg. MCP (₹/KWh)</t>
+          <t>Wt. Avg. MCP (₹/KWh)</t>
         </is>
       </c>
     </row>
@@ -913,7 +915,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4.999493541666666666666666667</t>
+          <t>4661.821206412914903017087805</t>
         </is>
       </c>
     </row>
@@ -925,7 +927,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4.999493541666666666666666667</t>
+          <t>3132.317546070094278926293971</t>
         </is>
       </c>
     </row>
@@ -937,7 +939,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5.323612083333333333333333333</t>
+          <t>4.523461626307502903644202927</t>
         </is>
       </c>
     </row>
@@ -949,7 +951,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5.323612083333333333333333333</t>
+          <t>4.800528670544235429364353883</t>
         </is>
       </c>
     </row>
@@ -961,7 +963,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>4.985656979166666666666666667</t>
+          <t>5.273936813374518488248408983</t>
         </is>
       </c>
     </row>
@@ -973,7 +975,213 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4.985656979166666666666666667</t>
+          <t>2.252347809248138012573027702</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Items</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Wt. Avg. MCP (₹/KWh)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>DAM 2024</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DAM 2023</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>GDAM 2024</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GDAM 2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>RTM 2024</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>RTM 2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Items</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Wt. Avg. MCP (₹/KWh)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>DAM 2024</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DAM 2023</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>GDAM 2024</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GDAM 2023</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>RTM 2024</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>RTM 2023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>